<commit_message>
update for new job
</commit_message>
<xml_diff>
--- a/A.XLSX
+++ b/A.XLSX
@@ -25,7 +25,7 @@
     <t>l25</t>
   </si>
   <si>
-    <t>l27</t>
+    <t>l27.6</t>
   </si>
 </sst>
 </file>
@@ -370,7 +370,7 @@
   <dimension ref="A1:D12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F5" sqref="F5"/>
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>

</xml_diff>

<commit_message>
new class for grafics
</commit_message>
<xml_diff>
--- a/A.XLSX
+++ b/A.XLSX
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="4">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7" uniqueCount="7">
   <si>
     <t>h</t>
   </si>
@@ -26,6 +26,15 @@
   </si>
   <si>
     <t>l27.6</t>
+  </si>
+  <si>
+    <t>l27</t>
+  </si>
+  <si>
+    <t>l25.0</t>
+  </si>
+  <si>
+    <t>l23.0</t>
   </si>
 </sst>
 </file>
@@ -367,15 +376,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D12"/>
+  <dimension ref="A1:G12"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D1" sqref="D1"/>
+      <selection activeCell="E2" sqref="E2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -388,8 +397,17 @@
       <c r="D1" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E1" t="s">
+        <v>6</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>20</v>
       </c>
@@ -402,8 +420,17 @@
       <c r="D2">
         <v>5.7000000000000002E-2</v>
       </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E2">
+        <v>4.5999999999999999E-2</v>
+      </c>
+      <c r="F2">
+        <v>5.0999999999999997E-2</v>
+      </c>
+      <c r="G2">
+        <v>5.7000000000000002E-2</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>25</v>
       </c>
@@ -416,8 +443,17 @@
       <c r="D3">
         <v>9.4E-2</v>
       </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E3">
+        <v>7.6999999999999999E-2</v>
+      </c>
+      <c r="F3">
+        <v>8.5000000000000006E-2</v>
+      </c>
+      <c r="G3">
+        <v>9.4E-2</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>30</v>
       </c>
@@ -430,8 +466,17 @@
       <c r="D4">
         <v>0.13400000000000001</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E4">
+        <v>0.11</v>
+      </c>
+      <c r="F4">
+        <v>0.122</v>
+      </c>
+      <c r="G4">
+        <v>0.13400000000000001</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>35</v>
       </c>
@@ -444,8 +489,17 @@
       <c r="D5">
         <v>0.17399999999999999</v>
       </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E5">
+        <v>0.14499999999999999</v>
+      </c>
+      <c r="F5">
+        <v>0.159</v>
+      </c>
+      <c r="G5">
+        <v>0.17399999999999999</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>40</v>
       </c>
@@ -458,8 +512,17 @@
       <c r="D6">
         <v>0.21099999999999999</v>
       </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E6">
+        <v>0.17599999999999999</v>
+      </c>
+      <c r="F6">
+        <v>0.19400000000000001</v>
+      </c>
+      <c r="G6">
+        <v>0.21099999999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>45</v>
       </c>
@@ -472,8 +535,17 @@
       <c r="D7">
         <v>0.24399999999999999</v>
       </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E7">
+        <v>0.20499999999999999</v>
+      </c>
+      <c r="F7">
+        <v>0.224</v>
+      </c>
+      <c r="G7">
+        <v>0.24399999999999999</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>50</v>
       </c>
@@ -486,8 +558,17 @@
       <c r="D8">
         <v>0.27200000000000002</v>
       </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E8">
+        <v>0.22900000000000001</v>
+      </c>
+      <c r="F8">
+        <v>0.25</v>
+      </c>
+      <c r="G8">
+        <v>0.27200000000000002</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>55</v>
       </c>
@@ -500,8 +581,17 @@
       <c r="D9">
         <v>0.29499999999999998</v>
       </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E9">
+        <v>0.248</v>
+      </c>
+      <c r="F9">
+        <v>0.27100000000000002</v>
+      </c>
+      <c r="G9">
+        <v>0.29499999999999998</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>60</v>
       </c>
@@ -514,8 +604,17 @@
       <c r="D10">
         <v>0.312</v>
       </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E10">
+        <v>0.26400000000000001</v>
+      </c>
+      <c r="F10">
+        <v>0.28799999999999998</v>
+      </c>
+      <c r="G10">
+        <v>0.312</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>65</v>
       </c>
@@ -528,8 +627,17 @@
       <c r="D11">
         <v>0.32500000000000001</v>
       </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.3">
+      <c r="E11">
+        <v>0.27600000000000002</v>
+      </c>
+      <c r="F11">
+        <v>0.3</v>
+      </c>
+      <c r="G11">
+        <v>0.32500000000000001</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>70</v>
       </c>
@@ -540,6 +648,15 @@
         <v>0.309</v>
       </c>
       <c r="D12">
+        <v>0.33500000000000002</v>
+      </c>
+      <c r="E12">
+        <v>0.28399999999999997</v>
+      </c>
+      <c r="F12">
+        <v>0.309</v>
+      </c>
+      <c r="G12">
         <v>0.33500000000000002</v>
       </c>
     </row>

</xml_diff>